<commit_message>
update to main.java and msExcel.java. Built and tested two methods to append to the excel test file. added JavaTESTBooks.xlsx to build - used for testing
</commit_message>
<xml_diff>
--- a/Docs/Virtual Machines.xlsx
+++ b/Docs/Virtual Machines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="4" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="365">
   <si>
     <t>VM1</t>
   </si>
@@ -1106,12 +1106,15 @@
   </si>
   <si>
     <t>AVM1085</t>
+  </si>
+  <si>
+    <t>Vmname</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1423,27 +1426,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1471,6 +1454,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1779,27 +1772,29 @@
   </sheetPr>
   <dimension ref="A1:M151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H87" sqref="H87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7265625" style="1" customWidth="1"/>
     <col min="7" max="7" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="18.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="24.85546875" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.28515625" style="1"/>
+    <col min="8" max="10" width="18.453125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20.54296875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="24.81640625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>364</v>
+      </c>
       <c r="B1" s="7" t="s">
         <v>150</v>
       </c>
@@ -1831,7 +1826,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -1862,7 +1857,7 @@
       </c>
       <c r="K2" s="10"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
@@ -1893,7 +1888,7 @@
       </c>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
@@ -1924,7 +1919,7 @@
       </c>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
@@ -1955,7 +1950,7 @@
       </c>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
@@ -1986,7 +1981,7 @@
       </c>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
@@ -2017,7 +2012,7 @@
       </c>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>6</v>
       </c>
@@ -2048,7 +2043,7 @@
       </c>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>7</v>
       </c>
@@ -2079,7 +2074,7 @@
       </c>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
@@ -2110,7 +2105,7 @@
       </c>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>9</v>
       </c>
@@ -2141,7 +2136,7 @@
       </c>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>10</v>
       </c>
@@ -2172,7 +2167,7 @@
       </c>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>11</v>
       </c>
@@ -2203,7 +2198,7 @@
       </c>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>12</v>
       </c>
@@ -2234,7 +2229,7 @@
       </c>
       <c r="K14" s="11"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>13</v>
       </c>
@@ -2265,7 +2260,7 @@
       </c>
       <c r="K15" s="10"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>14</v>
       </c>
@@ -2296,7 +2291,7 @@
       </c>
       <c r="K16" s="10"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>15</v>
       </c>
@@ -2327,7 +2322,7 @@
       </c>
       <c r="K17" s="10"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>16</v>
       </c>
@@ -2358,7 +2353,7 @@
       </c>
       <c r="K18" s="10"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>17</v>
       </c>
@@ -2389,7 +2384,7 @@
       </c>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>18</v>
       </c>
@@ -2420,7 +2415,7 @@
       </c>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>19</v>
       </c>
@@ -2451,7 +2446,7 @@
       </c>
       <c r="K21" s="10"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>20</v>
       </c>
@@ -2482,7 +2477,7 @@
       </c>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>21</v>
       </c>
@@ -2513,7 +2508,7 @@
       </c>
       <c r="K23" s="10"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>22</v>
       </c>
@@ -2544,7 +2539,7 @@
       </c>
       <c r="K24" s="10"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>23</v>
       </c>
@@ -2575,7 +2570,7 @@
       </c>
       <c r="K25" s="10"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
         <v>24</v>
       </c>
@@ -2606,7 +2601,7 @@
       </c>
       <c r="K26" s="10"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
         <v>25</v>
       </c>
@@ -2637,7 +2632,7 @@
       </c>
       <c r="K27" s="10"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
         <v>26</v>
       </c>
@@ -2670,7 +2665,7 @@
       </c>
       <c r="K28" s="10"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
         <v>27</v>
       </c>
@@ -2701,7 +2696,7 @@
       </c>
       <c r="K29" s="10"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
         <v>28</v>
       </c>
@@ -2732,7 +2727,7 @@
       </c>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
         <v>29</v>
       </c>
@@ -2763,7 +2758,7 @@
       </c>
       <c r="K31" s="10"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
         <v>30</v>
       </c>
@@ -2794,7 +2789,7 @@
       </c>
       <c r="K32" s="10"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
         <v>31</v>
       </c>
@@ -2825,7 +2820,7 @@
       </c>
       <c r="K33" s="10"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>32</v>
       </c>
@@ -2856,7 +2851,7 @@
       </c>
       <c r="K34" s="10"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
         <v>33</v>
       </c>
@@ -2887,7 +2882,7 @@
       </c>
       <c r="K35" s="10"/>
     </row>
-    <row r="36" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
         <v>34</v>
       </c>
@@ -2918,7 +2913,7 @@
       </c>
       <c r="K36" s="10"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
         <v>35</v>
       </c>
@@ -2949,7 +2944,7 @@
       </c>
       <c r="K37" s="10"/>
     </row>
-    <row r="38" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
         <v>36</v>
       </c>
@@ -2980,7 +2975,7 @@
       </c>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="18" t="s">
         <v>37</v>
       </c>
@@ -3019,7 +3014,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="18" t="s">
         <v>38</v>
       </c>
@@ -3058,7 +3053,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="18" t="s">
         <v>39</v>
       </c>
@@ -3097,7 +3092,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
         <v>40</v>
       </c>
@@ -3128,7 +3123,7 @@
       </c>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
         <v>41</v>
       </c>
@@ -3159,7 +3154,7 @@
       </c>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="9" t="s">
         <v>42</v>
       </c>
@@ -3190,7 +3185,7 @@
       </c>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>43</v>
       </c>
@@ -3221,7 +3216,7 @@
       </c>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
         <v>44</v>
       </c>
@@ -3252,7 +3247,7 @@
       </c>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
         <v>45</v>
       </c>
@@ -3283,7 +3278,7 @@
       </c>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
         <v>46</v>
       </c>
@@ -3314,7 +3309,7 @@
       </c>
       <c r="K48" s="10"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
         <v>47</v>
       </c>
@@ -3345,7 +3340,7 @@
       </c>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
         <v>48</v>
       </c>
@@ -3376,7 +3371,7 @@
       </c>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
         <v>49</v>
       </c>
@@ -3407,7 +3402,7 @@
       </c>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
         <v>50</v>
       </c>
@@ -3438,7 +3433,7 @@
       </c>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
         <v>51</v>
       </c>
@@ -3469,7 +3464,7 @@
       </c>
       <c r="K53" s="10"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" s="9" t="s">
         <v>52</v>
       </c>
@@ -3500,7 +3495,7 @@
       </c>
       <c r="K54" s="10"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
         <v>53</v>
       </c>
@@ -3531,7 +3526,7 @@
       </c>
       <c r="K55" s="10"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
         <v>54</v>
       </c>
@@ -3562,7 +3557,7 @@
       </c>
       <c r="K56" s="10"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
         <v>55</v>
       </c>
@@ -3593,7 +3588,7 @@
       </c>
       <c r="K57" s="10"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="s">
         <v>56</v>
       </c>
@@ -3624,7 +3619,7 @@
       </c>
       <c r="K58" s="10"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
         <v>57</v>
       </c>
@@ -3655,7 +3650,7 @@
       </c>
       <c r="K59" s="10"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" s="9" t="s">
         <v>58</v>
       </c>
@@ -3686,7 +3681,7 @@
       </c>
       <c r="K60" s="10"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
         <v>59</v>
       </c>
@@ -3717,7 +3712,7 @@
       </c>
       <c r="K61" s="10"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
         <v>60</v>
       </c>
@@ -3748,7 +3743,7 @@
       </c>
       <c r="K62" s="10"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
         <v>61</v>
       </c>
@@ -3779,7 +3774,7 @@
       </c>
       <c r="K63" s="10"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" s="9" t="s">
         <v>62</v>
       </c>
@@ -3810,7 +3805,7 @@
       </c>
       <c r="K64" s="10"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" s="9" t="s">
         <v>63</v>
       </c>
@@ -3841,7 +3836,7 @@
       </c>
       <c r="K65" s="10"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
         <v>64</v>
       </c>
@@ -3872,7 +3867,7 @@
       </c>
       <c r="K66" s="10"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" s="9" t="s">
         <v>65</v>
       </c>
@@ -3903,7 +3898,7 @@
       </c>
       <c r="K67" s="10"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" s="19" t="s">
         <v>66</v>
       </c>
@@ -3934,7 +3929,7 @@
       </c>
       <c r="K68" s="10"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" s="19" t="s">
         <v>67</v>
       </c>
@@ -3965,7 +3960,7 @@
       </c>
       <c r="K69" s="10"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" s="18" t="s">
         <v>68</v>
       </c>
@@ -3998,7 +3993,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" s="18" t="s">
         <v>69</v>
       </c>
@@ -4031,7 +4026,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" s="18" t="s">
         <v>70</v>
       </c>
@@ -4064,7 +4059,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" s="18" t="s">
         <v>71</v>
       </c>
@@ -4097,7 +4092,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74" s="18" t="s">
         <v>72</v>
       </c>
@@ -4130,7 +4125,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75" s="18" t="s">
         <v>73</v>
       </c>
@@ -4163,7 +4158,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" s="18" t="s">
         <v>74</v>
       </c>
@@ -4196,7 +4191,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77" s="18" t="s">
         <v>75</v>
       </c>
@@ -4229,7 +4224,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78" s="9" t="s">
         <v>76</v>
       </c>
@@ -4260,7 +4255,7 @@
       </c>
       <c r="K78" s="10"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79" s="9" t="s">
         <v>77</v>
       </c>
@@ -4291,7 +4286,7 @@
       </c>
       <c r="K79" s="10"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80" s="9" t="s">
         <v>78</v>
       </c>
@@ -4322,7 +4317,7 @@
       </c>
       <c r="K80" s="10"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" s="9" t="s">
         <v>79</v>
       </c>
@@ -4353,7 +4348,7 @@
       </c>
       <c r="K81" s="10"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" s="9" t="s">
         <v>80</v>
       </c>
@@ -4384,7 +4379,7 @@
       </c>
       <c r="K82" s="10"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" s="9" t="s">
         <v>81</v>
       </c>
@@ -4415,7 +4410,7 @@
       </c>
       <c r="K83" s="10"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" s="9" t="s">
         <v>82</v>
       </c>
@@ -4446,7 +4441,7 @@
       </c>
       <c r="K84" s="10"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" s="9" t="s">
         <v>83</v>
       </c>
@@ -4477,7 +4472,7 @@
       </c>
       <c r="K85" s="10"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" s="9" t="s">
         <v>84</v>
       </c>
@@ -4508,7 +4503,7 @@
       </c>
       <c r="K86" s="10"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" s="9" t="s">
         <v>85</v>
       </c>
@@ -4523,7 +4518,7 @@
       <c r="J87" s="3"/>
       <c r="K87" s="10"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" s="9" t="s">
         <v>86</v>
       </c>
@@ -4538,7 +4533,7 @@
       <c r="J88" s="3"/>
       <c r="K88" s="10"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" s="9" t="s">
         <v>87</v>
       </c>
@@ -4553,7 +4548,7 @@
       <c r="J89" s="3"/>
       <c r="K89" s="10"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" s="9" t="s">
         <v>88</v>
       </c>
@@ -4568,7 +4563,7 @@
       <c r="J90" s="3"/>
       <c r="K90" s="10"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" s="9" t="s">
         <v>89</v>
       </c>
@@ -4583,7 +4578,7 @@
       <c r="J91" s="3"/>
       <c r="K91" s="10"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" s="9" t="s">
         <v>90</v>
       </c>
@@ -4598,7 +4593,7 @@
       <c r="J92" s="3"/>
       <c r="K92" s="10"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" s="9" t="s">
         <v>91</v>
       </c>
@@ -4613,7 +4608,7 @@
       <c r="J93" s="3"/>
       <c r="K93" s="10"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" s="9" t="s">
         <v>92</v>
       </c>
@@ -4628,7 +4623,7 @@
       <c r="J94" s="3"/>
       <c r="K94" s="10"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" s="9" t="s">
         <v>93</v>
       </c>
@@ -4643,7 +4638,7 @@
       <c r="J95" s="3"/>
       <c r="K95" s="10"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" s="9" t="s">
         <v>94</v>
       </c>
@@ -4658,7 +4653,7 @@
       <c r="J96" s="3"/>
       <c r="K96" s="10"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" s="9" t="s">
         <v>95</v>
       </c>
@@ -4673,7 +4668,7 @@
       <c r="J97" s="3"/>
       <c r="K97" s="10"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" s="9" t="s">
         <v>96</v>
       </c>
@@ -4688,7 +4683,7 @@
       <c r="J98" s="3"/>
       <c r="K98" s="10"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" s="9" t="s">
         <v>97</v>
       </c>
@@ -4703,7 +4698,7 @@
       <c r="J99" s="3"/>
       <c r="K99" s="10"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" s="9" t="s">
         <v>98</v>
       </c>
@@ -4718,7 +4713,7 @@
       <c r="J100" s="3"/>
       <c r="K100" s="10"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101" s="9" t="s">
         <v>99</v>
       </c>
@@ -4733,7 +4728,7 @@
       <c r="J101" s="3"/>
       <c r="K101" s="10"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A102" s="9" t="s">
         <v>100</v>
       </c>
@@ -4748,7 +4743,7 @@
       <c r="J102" s="3"/>
       <c r="K102" s="10"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A103" s="9" t="s">
         <v>101</v>
       </c>
@@ -4763,7 +4758,7 @@
       <c r="J103" s="3"/>
       <c r="K103" s="10"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104" s="9" t="s">
         <v>102</v>
       </c>
@@ -4778,7 +4773,7 @@
       <c r="J104" s="3"/>
       <c r="K104" s="10"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A105" s="9" t="s">
         <v>103</v>
       </c>
@@ -4793,7 +4788,7 @@
       <c r="J105" s="3"/>
       <c r="K105" s="10"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A106" s="9" t="s">
         <v>104</v>
       </c>
@@ -4808,7 +4803,7 @@
       <c r="J106" s="3"/>
       <c r="K106" s="10"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A107" s="9" t="s">
         <v>105</v>
       </c>
@@ -4823,7 +4818,7 @@
       <c r="J107" s="3"/>
       <c r="K107" s="10"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A108" s="9" t="s">
         <v>106</v>
       </c>
@@ -4838,7 +4833,7 @@
       <c r="J108" s="3"/>
       <c r="K108" s="10"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A109" s="9" t="s">
         <v>107</v>
       </c>
@@ -4853,7 +4848,7 @@
       <c r="J109" s="3"/>
       <c r="K109" s="10"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A110" s="9" t="s">
         <v>108</v>
       </c>
@@ -4868,7 +4863,7 @@
       <c r="J110" s="3"/>
       <c r="K110" s="10"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A111" s="9" t="s">
         <v>109</v>
       </c>
@@ -4883,7 +4878,7 @@
       <c r="J111" s="3"/>
       <c r="K111" s="10"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A112" s="9" t="s">
         <v>110</v>
       </c>
@@ -4898,7 +4893,7 @@
       <c r="J112" s="3"/>
       <c r="K112" s="10"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A113" s="9" t="s">
         <v>111</v>
       </c>
@@ -4913,7 +4908,7 @@
       <c r="J113" s="3"/>
       <c r="K113" s="10"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A114" s="9" t="s">
         <v>112</v>
       </c>
@@ -4928,7 +4923,7 @@
       <c r="J114" s="3"/>
       <c r="K114" s="10"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A115" s="9" t="s">
         <v>113</v>
       </c>
@@ -4943,7 +4938,7 @@
       <c r="J115" s="3"/>
       <c r="K115" s="10"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A116" s="9" t="s">
         <v>114</v>
       </c>
@@ -4958,7 +4953,7 @@
       <c r="J116" s="3"/>
       <c r="K116" s="10"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A117" s="9" t="s">
         <v>115</v>
       </c>
@@ -4973,7 +4968,7 @@
       <c r="J117" s="3"/>
       <c r="K117" s="10"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A118" s="9" t="s">
         <v>116</v>
       </c>
@@ -4988,7 +4983,7 @@
       <c r="J118" s="3"/>
       <c r="K118" s="10"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A119" s="9" t="s">
         <v>117</v>
       </c>
@@ -5003,7 +4998,7 @@
       <c r="J119" s="3"/>
       <c r="K119" s="10"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A120" s="9" t="s">
         <v>118</v>
       </c>
@@ -5018,7 +5013,7 @@
       <c r="J120" s="3"/>
       <c r="K120" s="10"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A121" s="9" t="s">
         <v>119</v>
       </c>
@@ -5033,7 +5028,7 @@
       <c r="J121" s="3"/>
       <c r="K121" s="10"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A122" s="9" t="s">
         <v>120</v>
       </c>
@@ -5048,7 +5043,7 @@
       <c r="J122" s="3"/>
       <c r="K122" s="10"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A123" s="9" t="s">
         <v>121</v>
       </c>
@@ -5063,7 +5058,7 @@
       <c r="J123" s="3"/>
       <c r="K123" s="10"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A124" s="9" t="s">
         <v>122</v>
       </c>
@@ -5078,7 +5073,7 @@
       <c r="J124" s="3"/>
       <c r="K124" s="10"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A125" s="9" t="s">
         <v>123</v>
       </c>
@@ -5093,7 +5088,7 @@
       <c r="J125" s="3"/>
       <c r="K125" s="10"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A126" s="9" t="s">
         <v>124</v>
       </c>
@@ -5108,7 +5103,7 @@
       <c r="J126" s="3"/>
       <c r="K126" s="10"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A127" s="9" t="s">
         <v>125</v>
       </c>
@@ -5123,7 +5118,7 @@
       <c r="J127" s="3"/>
       <c r="K127" s="10"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A128" s="9" t="s">
         <v>126</v>
       </c>
@@ -5138,7 +5133,7 @@
       <c r="J128" s="3"/>
       <c r="K128" s="10"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A129" s="9" t="s">
         <v>127</v>
       </c>
@@ -5153,7 +5148,7 @@
       <c r="J129" s="3"/>
       <c r="K129" s="10"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A130" s="9" t="s">
         <v>128</v>
       </c>
@@ -5168,7 +5163,7 @@
       <c r="J130" s="3"/>
       <c r="K130" s="10"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A131" s="9" t="s">
         <v>129</v>
       </c>
@@ -5183,7 +5178,7 @@
       <c r="J131" s="3"/>
       <c r="K131" s="10"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A132" s="9" t="s">
         <v>130</v>
       </c>
@@ -5198,7 +5193,7 @@
       <c r="J132" s="3"/>
       <c r="K132" s="10"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A133" s="9" t="s">
         <v>131</v>
       </c>
@@ -5213,7 +5208,7 @@
       <c r="J133" s="3"/>
       <c r="K133" s="10"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A134" s="9" t="s">
         <v>132</v>
       </c>
@@ -5228,7 +5223,7 @@
       <c r="J134" s="3"/>
       <c r="K134" s="10"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A135" s="9" t="s">
         <v>133</v>
       </c>
@@ -5243,7 +5238,7 @@
       <c r="J135" s="3"/>
       <c r="K135" s="10"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A136" s="9" t="s">
         <v>134</v>
       </c>
@@ -5258,7 +5253,7 @@
       <c r="J136" s="3"/>
       <c r="K136" s="10"/>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A137" s="9" t="s">
         <v>135</v>
       </c>
@@ -5273,7 +5268,7 @@
       <c r="J137" s="3"/>
       <c r="K137" s="10"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A138" s="9" t="s">
         <v>136</v>
       </c>
@@ -5288,7 +5283,7 @@
       <c r="J138" s="3"/>
       <c r="K138" s="10"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A139" s="9" t="s">
         <v>137</v>
       </c>
@@ -5303,7 +5298,7 @@
       <c r="J139" s="3"/>
       <c r="K139" s="10"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A140" s="9" t="s">
         <v>138</v>
       </c>
@@ -5318,7 +5313,7 @@
       <c r="J140" s="3"/>
       <c r="K140" s="10"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A141" s="9" t="s">
         <v>139</v>
       </c>
@@ -5333,7 +5328,7 @@
       <c r="J141" s="3"/>
       <c r="K141" s="10"/>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A142" s="9" t="s">
         <v>140</v>
       </c>
@@ -5348,7 +5343,7 @@
       <c r="J142" s="3"/>
       <c r="K142" s="10"/>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A143" s="9" t="s">
         <v>141</v>
       </c>
@@ -5363,7 +5358,7 @@
       <c r="J143" s="3"/>
       <c r="K143" s="10"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A144" s="9" t="s">
         <v>142</v>
       </c>
@@ -5378,7 +5373,7 @@
       <c r="J144" s="3"/>
       <c r="K144" s="10"/>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A145" s="9" t="s">
         <v>143</v>
       </c>
@@ -5393,7 +5388,7 @@
       <c r="J145" s="3"/>
       <c r="K145" s="10"/>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A146" s="9" t="s">
         <v>144</v>
       </c>
@@ -5408,7 +5403,7 @@
       <c r="J146" s="3"/>
       <c r="K146" s="10"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A147" s="9" t="s">
         <v>145</v>
       </c>
@@ -5423,7 +5418,7 @@
       <c r="J147" s="3"/>
       <c r="K147" s="10"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A148" s="9" t="s">
         <v>146</v>
       </c>
@@ -5438,7 +5433,7 @@
       <c r="J148" s="3"/>
       <c r="K148" s="10"/>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A149" s="9" t="s">
         <v>147</v>
       </c>
@@ -5453,7 +5448,7 @@
       <c r="J149" s="3"/>
       <c r="K149" s="10"/>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A150" s="9" t="s">
         <v>148</v>
       </c>
@@ -5468,7 +5463,7 @@
       <c r="J150" s="3"/>
       <c r="K150" s="10"/>
     </row>
-    <row r="151" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A151" s="12" t="s">
         <v>149</v>
       </c>
@@ -5485,18 +5480,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"LiveCHS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"LiveFRN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="66" fitToHeight="7" orientation="landscape" r:id="rId1"/>

</xml_diff>